<commit_message>
Yang Li put his name
</commit_message>
<xml_diff>
--- a/GitTest.xlsx
+++ b/GitTest.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="110" windowWidth="14810" windowHeight="8010"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="21570" windowHeight="7545"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="5">
   <si>
     <t>Name</t>
   </si>
@@ -26,6 +26,9 @@
   </si>
   <si>
     <t>Yes</t>
+  </si>
+  <si>
+    <t>Yang Li</t>
   </si>
 </sst>
 </file>
@@ -367,15 +370,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B2"/>
+  <dimension ref="A1:B3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -383,11 +386,19 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>2</v>
       </c>
       <c r="B2" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>4</v>
+      </c>
+      <c r="B3" t="s">
         <v>3</v>
       </c>
     </row>

</xml_diff>